<commit_message>
17.05.2024 - ekran son halini aldı ve sistem test edildi.
</commit_message>
<xml_diff>
--- a/doc/IO_List.XLSX
+++ b/doc/IO_List.XLSX
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MSE_Proje\Mersin\MSE.Mersin.Kenetleme\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF9D364C-EA3C-4A07-B0E4-4FF7F3141504}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F53B408-1604-42F0-B42A-A2041AAB55FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="840" yWindow="420" windowWidth="26910" windowHeight="14835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="84">
   <si>
     <t>Tanım</t>
   </si>
@@ -114,24 +114,12 @@
     <t>P3_geride</t>
   </si>
   <si>
-    <t>P3A_ileride</t>
-  </si>
-  <si>
-    <t>P3A_geride</t>
-  </si>
-  <si>
     <t>P4_ileride</t>
   </si>
   <si>
     <t>P4_geride</t>
   </si>
   <si>
-    <t>P4A_ileride</t>
-  </si>
-  <si>
-    <t>P4A_geride</t>
-  </si>
-  <si>
     <t>i2.0</t>
   </si>
   <si>
@@ -150,30 +138,6 @@
     <t>i2.5</t>
   </si>
   <si>
-    <t>i2.6</t>
-  </si>
-  <si>
-    <t>i2.7</t>
-  </si>
-  <si>
-    <t>p4b_ileride</t>
-  </si>
-  <si>
-    <t>p4b_geride</t>
-  </si>
-  <si>
-    <t>P4C_ileride</t>
-  </si>
-  <si>
-    <t>P4C_geride</t>
-  </si>
-  <si>
-    <t>Vinc_Lambasi</t>
-  </si>
-  <si>
-    <t>i3.0</t>
-  </si>
-  <si>
     <t>PLC Output Adresi</t>
   </si>
   <si>
@@ -198,18 +162,12 @@
     <t>Vinc Lambasi</t>
   </si>
   <si>
-    <t>i3.1</t>
-  </si>
-  <si>
     <t>Kırmızı</t>
   </si>
   <si>
     <t>Vakum</t>
   </si>
   <si>
-    <t>i3.2</t>
-  </si>
-  <si>
     <t>i3.6</t>
   </si>
   <si>
@@ -234,29 +192,98 @@
     <t>Q0.0</t>
   </si>
   <si>
-    <t xml:space="preserve">p4  ileride </t>
-  </si>
-  <si>
-    <t xml:space="preserve">p4 geride </t>
-  </si>
-  <si>
-    <t>p4b ileri</t>
-  </si>
-  <si>
-    <t>p4b geri</t>
-  </si>
-  <si>
-    <t>Vinc_Lambası</t>
-  </si>
-  <si>
-    <t>Servo Home</t>
+    <t>Q4.0</t>
+  </si>
+  <si>
+    <t>Q4.1</t>
+  </si>
+  <si>
+    <t>Q4.2</t>
+  </si>
+  <si>
+    <t>Q4.3</t>
+  </si>
+  <si>
+    <t>Q4.4</t>
+  </si>
+  <si>
+    <t>Q4.5</t>
+  </si>
+  <si>
+    <t>Q4.6</t>
+  </si>
+  <si>
+    <t>Q4.7</t>
+  </si>
+  <si>
+    <t>Q5.1</t>
+  </si>
+  <si>
+    <t>Q5.0</t>
+  </si>
+  <si>
+    <t>Festo I/O (Profinet)</t>
+  </si>
+  <si>
+    <t>P4B (Sol)- Geri</t>
+  </si>
+  <si>
+    <t>Konum</t>
+  </si>
+  <si>
+    <t>P4B (Sol)- İleri</t>
+  </si>
+  <si>
+    <t>P4 (Sağ)- Geri</t>
+  </si>
+  <si>
+    <t>P4 (Sağ)- İleri</t>
+  </si>
+  <si>
+    <t>P1/P1A - Geri</t>
+  </si>
+  <si>
+    <t>P1/P1A - İleri</t>
+  </si>
+  <si>
+    <t>P2/P2A - Geri</t>
+  </si>
+  <si>
+    <t>P2/P2A - İleri</t>
+  </si>
+  <si>
+    <t>P3 - Geri</t>
+  </si>
+  <si>
+    <t>P3 - İleri</t>
+  </si>
+  <si>
+    <t>Kadem Pis.</t>
+  </si>
+  <si>
+    <t>Model Pis.</t>
+  </si>
+  <si>
+    <t>Kenetleme Pis.</t>
+  </si>
+  <si>
+    <t>P4B_ileride</t>
+  </si>
+  <si>
+    <t>P4B_geride</t>
+  </si>
+  <si>
+    <t>Vinc lambası</t>
+  </si>
+  <si>
+    <t>Servo home sen.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -297,8 +324,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -339,6 +372,18 @@
         <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -369,7 +414,7 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -383,7 +428,6 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -396,10 +440,18 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -682,17 +734,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C41"/>
+  <dimension ref="A1:C48"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R30" sqref="R30"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39.85546875" customWidth="1"/>
-    <col min="2" max="2" width="28.28515625" customWidth="1"/>
-    <col min="3" max="3" width="19" customWidth="1"/>
+    <col min="1" max="1" width="33" customWidth="1"/>
+    <col min="2" max="2" width="22.5703125" customWidth="1"/>
+    <col min="3" max="3" width="20.140625" customWidth="1"/>
     <col min="4" max="4" width="12.85546875" customWidth="1"/>
     <col min="5" max="5" width="12.7109375" customWidth="1"/>
     <col min="6" max="7" width="10.7109375" customWidth="1"/>
@@ -718,7 +770,7 @@
     </row>
     <row r="3" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>4</v>
@@ -829,197 +881,267 @@
         <v>29</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C17" s="11" t="s">
-        <v>69</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="C17" s="13"/>
     </row>
     <row r="18" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="10" t="s">
+      <c r="A18" s="12" t="s">
         <v>30</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C18" s="11" t="s">
-        <v>70</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="C18" s="13"/>
     </row>
     <row r="19" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="5"/>
+      <c r="A19" s="11"/>
       <c r="B19" s="3"/>
+      <c r="C19" s="14"/>
     </row>
     <row r="20" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="10" t="s">
-        <v>31</v>
+      <c r="A20" s="12" t="s">
+        <v>80</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C20" s="11" t="s">
-        <v>71</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="C20" s="13"/>
     </row>
     <row r="21" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="10" t="s">
-        <v>32</v>
+        <v>81</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C21" s="11" t="s">
-        <v>72</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="C21" s="13"/>
     </row>
     <row r="22" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="10" t="s">
-        <v>33</v>
+      <c r="A22" s="12" t="s">
+        <v>82</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="C22" s="11" t="s">
-        <v>73</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="C22" s="13"/>
     </row>
     <row r="23" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="10" t="s">
-        <v>34</v>
+        <v>83</v>
       </c>
       <c r="B23" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C23" s="13"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="6"/>
+      <c r="B24" s="6"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="1"/>
+    </row>
+    <row r="29" spans="1:3" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B32" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C23" s="11" t="s">
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="6"/>
+      <c r="B36" s="6"/>
+    </row>
+    <row r="38" spans="1:3" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="B39" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="C39" s="9" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="B41" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="C41" s="9" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="B43" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="C43" s="9" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="B45" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="C45" s="9" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B46" s="1" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A27" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A28" s="5"/>
-      <c r="B28" s="3"/>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="B29" s="6" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="7" t="s">
+      <c r="C46" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="B47" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="C47" s="9" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B30" s="7" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="B31" s="9" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="1"/>
-      <c r="B32" s="1"/>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="1"/>
-    </row>
-    <row r="34" spans="1:2" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="A34" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="B35" s="7" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="B36" s="6" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="B37" s="7" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="B38" s="6" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="B39" s="7" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="B40" s="6" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="7"/>
-      <c r="B41" s="7"/>
+      <c r="B48" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>77</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>